<commit_message>
Removed quotes from json bug data. Added function to lookup bug information by bug name.
</commit_message>
<xml_diff>
--- a/critters.xlsx
+++ b/critters.xlsx
@@ -488,24 +488,6 @@
     <t>Scorpion</t>
   </si>
   <si>
-    <t xml:space="preserve">, "name": </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ "id": </t>
-  </si>
-  <si>
-    <t xml:space="preserve">, "type": </t>
-  </si>
-  <si>
-    <t xml:space="preserve">, "value": </t>
-  </si>
-  <si>
-    <t xml:space="preserve">, "time": </t>
-  </si>
-  <si>
-    <t xml:space="preserve">, "season": </t>
-  </si>
-  <si>
     <t xml:space="preserve"> },</t>
   </si>
   <si>
@@ -513,6 +495,24 @@
   </si>
   <si>
     <t>];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, name: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ id: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, type: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, value: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, time: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">, season: </t>
   </si>
 </sst>
 </file>
@@ -841,7 +841,7 @@
   <dimension ref="A1:R84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,31 +856,31 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="H1" t="s">
+        <v>155</v>
+      </c>
+      <c r="J1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L1" t="s">
+        <v>159</v>
+      </c>
+      <c r="M1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N1" t="s">
         <v>161</v>
       </c>
-      <c r="J1" t="s">
-        <v>155</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
+        <v>162</v>
+      </c>
+      <c r="P1" t="s">
         <v>154</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>156</v>
-      </c>
-      <c r="M1" t="s">
-        <v>157</v>
-      </c>
-      <c r="N1" t="s">
-        <v>158</v>
-      </c>
-      <c r="O1" t="s">
-        <v>159</v>
-      </c>
-      <c r="P1" t="s">
-        <v>160</v>
-      </c>
-      <c r="R1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -911,27 +911,27 @@
       </c>
       <c r="J4" t="str">
         <f>J$1&amp;A4</f>
-        <v>{ "id": 1</v>
+        <v>{ id: 1</v>
       </c>
       <c r="K4" t="str">
         <f>K$1&amp;""""&amp;B4&amp;""""</f>
-        <v>, "name": "Common Butterfly"</v>
+        <v>, name: "Common Butterfly"</v>
       </c>
       <c r="L4" t="str">
         <f>L$1&amp;""""&amp;C4&amp;""""</f>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M4" t="str">
         <f>M$1&amp;D4</f>
-        <v>, "value": 160</v>
+        <v>, value: 160</v>
       </c>
       <c r="N4" t="str">
         <f>N$1&amp;""""&amp;E4&amp;""""</f>
-        <v>, "time": "4 a.m. - 7 p.m."</v>
+        <v>, time: "4 a.m. - 7 p.m."</v>
       </c>
       <c r="O4" t="str">
         <f>O$1&amp;""""&amp;F4&amp;""""</f>
-        <v>, "season": "September-June (Northern) / March-December (Southern)"</v>
+        <v>, season: "September-June (Northern) / March-December (Southern)"</v>
       </c>
       <c r="P4" t="str">
         <f>P$1</f>
@@ -940,7 +940,7 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2" t="str">
         <f>J4&amp;K4&amp;L4&amp;M4&amp;N4&amp;O4&amp;P4</f>
-        <v>{ "id": 1, "name": "Common Butterfly", "type": "Flying", "value": 160, "time": "4 a.m. - 7 p.m.", "season": "September-June (Northern) / March-December (Southern)" },</v>
+        <v>{ id: 1, name: "Common Butterfly", type: "Flying", value: 160, time: "4 a.m. - 7 p.m.", season: "September-June (Northern) / March-December (Southern)" },</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -964,27 +964,27 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" ref="J5:J68" si="0">J$1&amp;A5</f>
-        <v>{ "id": 2</v>
+        <v>{ id: 2</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K68" si="1">K$1&amp;""""&amp;B5&amp;""""</f>
-        <v>, "name": "Yellow Butterfly"</v>
+        <v>, name: "Yellow Butterfly"</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ref="L5:L68" si="2">L$1&amp;""""&amp;C5&amp;""""</f>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ref="M5:M68" si="3">M$1&amp;D5</f>
-        <v>, "value": 160</v>
+        <v>, value: 160</v>
       </c>
       <c r="N5" t="str">
         <f t="shared" ref="N5:N68" si="4">N$1&amp;""""&amp;E5&amp;""""</f>
-        <v>, "time": "4 a.m. - 7 p.m."</v>
+        <v>, time: "4 a.m. - 7 p.m."</v>
       </c>
       <c r="O5" t="str">
         <f t="shared" ref="O5:O68" si="5">O$1&amp;""""&amp;F5&amp;""""</f>
-        <v>, "season": "March-June, September-October (Northern) / March-April, September-December (Southern)"</v>
+        <v>, season: "March-June, September-October (Northern) / March-April, September-December (Southern)"</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" ref="P5:P68" si="6">P$1</f>
@@ -993,7 +993,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2" t="str">
         <f t="shared" ref="R5:R68" si="7">J5&amp;K5&amp;L5&amp;M5&amp;N5&amp;O5&amp;P5</f>
-        <v>{ "id": 2, "name": "Yellow Butterfly", "type": "Flying", "value": 160, "time": "4 a.m. - 7 p.m.", "season": "March-June, September-October (Northern) / March-April, September-December (Southern)" },</v>
+        <v>{ id: 2, name: "Yellow Butterfly", type: "Flying", value: 160, time: "4 a.m. - 7 p.m.", season: "March-June, September-October (Northern) / March-April, September-December (Southern)" },</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1017,27 +1017,27 @@
       </c>
       <c r="J6" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 3</v>
+        <v>{ id: 3</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Tiger Butterfly"</v>
+        <v>, name: "Tiger Butterfly"</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 240</v>
+        <v>, value: 240</v>
       </c>
       <c r="N6" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "4 a.m. - 7 p.m."</v>
+        <v>, time: "4 a.m. - 7 p.m."</v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "March-September (Northern) / September-March (Southern)"</v>
+        <v>, season: "March-September (Northern) / September-March (Southern)"</v>
       </c>
       <c r="P6" t="str">
         <f t="shared" si="6"/>
@@ -1046,7 +1046,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 3, "name": "Tiger Butterfly", "type": "Flying", "value": 240, "time": "4 a.m. - 7 p.m.", "season": "March-September (Northern) / September-March (Southern)" },</v>
+        <v>{ id: 3, name: "Tiger Butterfly", type: "Flying", value: 240, time: "4 a.m. - 7 p.m.", season: "March-September (Northern) / September-March (Southern)" },</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1070,27 +1070,27 @@
       </c>
       <c r="J7" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 4</v>
+        <v>{ id: 4</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Peacock Butterfly"</v>
+        <v>, name: "Peacock Butterfly"</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying by hybrid flowers"</v>
+        <v>, type: "Flying by hybrid flowers"</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 2500</v>
+        <v>, value: 2500</v>
       </c>
       <c r="N7" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "4 a.m. - 7 p.m."</v>
+        <v>, time: "4 a.m. - 7 p.m."</v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "March-June (Northern) / September-December (Southern)"</v>
+        <v>, season: "March-June (Northern) / September-December (Southern)"</v>
       </c>
       <c r="P7" t="str">
         <f t="shared" si="6"/>
@@ -1099,7 +1099,7 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 4, "name": "Peacock Butterfly", "type": "Flying by hybrid flowers", "value": 2500, "time": "4 a.m. - 7 p.m.", "season": "March-June (Northern) / September-December (Southern)" },</v>
+        <v>{ id: 4, name: "Peacock Butterfly", type: "Flying by hybrid flowers", value: 2500, time: "4 a.m. - 7 p.m.", season: "March-June (Northern) / September-December (Southern)" },</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1123,27 +1123,27 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 5</v>
+        <v>{ id: 5</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Common Bluebottle"</v>
+        <v>, name: "Common Bluebottle"</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 300</v>
+        <v>, value: 300</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "4 a.m. - 7 p.m."</v>
+        <v>, time: "4 a.m. - 7 p.m."</v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-August (Northern) / October-February (Southern)"</v>
+        <v>, season: "April-August (Northern) / October-February (Southern)"</v>
       </c>
       <c r="P8" t="str">
         <f t="shared" si="6"/>
@@ -1152,7 +1152,7 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 5, "name": "Common Bluebottle", "type": "Flying", "value": 300, "time": "4 a.m. - 7 p.m.", "season": "April-August (Northern) / October-February (Southern)" },</v>
+        <v>{ id: 5, name: "Common Bluebottle", type: "Flying", value: 300, time: "4 a.m. - 7 p.m.", season: "April-August (Northern) / October-February (Southern)" },</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1176,27 +1176,27 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 6</v>
+        <v>{ id: 6</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Paper Kite Butterfly"</v>
+        <v>, name: "Paper Kite Butterfly"</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 1000</v>
+        <v>, value: 1000</v>
       </c>
       <c r="N9" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 7 p.m."</v>
+        <v>, time: "8 a.m. - 7 p.m."</v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" si="6"/>
@@ -1205,7 +1205,7 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 6, "name": "Paper Kite Butterfly", "type": "Flying", "value": 1000, "time": "8 a.m. - 7 p.m.", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 6, name: "Paper Kite Butterfly", type: "Flying", value: 1000, time: "8 a.m. - 7 p.m.", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1229,27 +1229,27 @@
       </c>
       <c r="J10" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 7</v>
+        <v>{ id: 7</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Great Purple Emperor"</v>
+        <v>, name: "Great Purple Emperor"</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 3000</v>
+        <v>, value: 3000</v>
       </c>
       <c r="N10" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "4 a.m. - 7 p.m."</v>
+        <v>, time: "4 a.m. - 7 p.m."</v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "May-August (Northern) / November-February (Southern)"</v>
+        <v>, season: "May-August (Northern) / November-February (Southern)"</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="6"/>
@@ -1258,7 +1258,7 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 7, "name": "Great Purple Emperor", "type": "Flying", "value": 3000, "time": "4 a.m. - 7 p.m.", "season": "May-August (Northern) / November-February (Southern)" },</v>
+        <v>{ id: 7, name: "Great Purple Emperor", type: "Flying", value: 3000, time: "4 a.m. - 7 p.m.", season: "May-August (Northern) / November-February (Southern)" },</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1282,27 +1282,27 @@
       </c>
       <c r="J11" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 8</v>
+        <v>{ id: 8</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Monach Butterfly"</v>
+        <v>, name: "Monach Butterfly"</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 140</v>
+        <v>, value: 140</v>
       </c>
       <c r="N11" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "4 a.m. - 5 p.m."</v>
+        <v>, time: "4 a.m. - 5 p.m."</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "September-November (Northern) / March-May (Southern)"</v>
+        <v>, season: "September-November (Northern) / March-May (Southern)"</v>
       </c>
       <c r="P11" t="str">
         <f t="shared" si="6"/>
@@ -1311,7 +1311,7 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 8, "name": "Monach Butterfly", "type": "Flying", "value": 140, "time": "4 a.m. - 5 p.m.", "season": "September-November (Northern) / March-May (Southern)" },</v>
+        <v>{ id: 8, name: "Monach Butterfly", type: "Flying", value: 140, time: "4 a.m. - 5 p.m.", season: "September-November (Northern) / March-May (Southern)" },</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -1335,27 +1335,27 @@
       </c>
       <c r="J12" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 9</v>
+        <v>{ id: 9</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Emperor Butterfly"</v>
+        <v>, name: "Emperor Butterfly"</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 4000</v>
+        <v>, value: 4000</v>
       </c>
       <c r="N12" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "June-September, December-March (Northern) / December-March, June-September (Southern)"</v>
+        <v>, season: "June-September, December-March (Northern) / December-March, June-September (Southern)"</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" si="6"/>
@@ -1364,7 +1364,7 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 9, "name": "Emperor Butterfly", "type": "Flying", "value": 4000, "time": "5 p.m. - 8 a.m.", "season": "June-September, December-March (Northern) / December-March, June-September (Southern)" },</v>
+        <v>{ id: 9, name: "Emperor Butterfly", type: "Flying", value: 4000, time: "5 p.m. - 8 a.m.", season: "June-September, December-March (Northern) / December-March, June-September (Southern)" },</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -1388,27 +1388,27 @@
       </c>
       <c r="J13" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 10</v>
+        <v>{ id: 10</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Agrias Butterfly"</v>
+        <v>, name: "Agrias Butterfly"</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 3000</v>
+        <v>, value: 3000</v>
       </c>
       <c r="N13" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-September (Northern) / November-March (Southern)"</v>
+        <v>, season: "April-September (Northern) / November-March (Southern)"</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="6"/>
@@ -1417,7 +1417,7 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 10, "name": "Agrias Butterfly", "type": "Flying", "value": 3000, "time": "8 a.m. - 5 p.m.", "season": "April-September (Northern) / November-March (Southern)" },</v>
+        <v>{ id: 10, name: "Agrias Butterfly", type: "Flying", value: 3000, time: "8 a.m. - 5 p.m.", season: "April-September (Northern) / November-March (Southern)" },</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -1441,27 +1441,27 @@
       </c>
       <c r="J14" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 11</v>
+        <v>{ id: 11</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Raja Brooke's Birdwing"</v>
+        <v>, name: "Raja Brooke's Birdwing"</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying by purple flowers"</v>
+        <v>, type: "Flying by purple flowers"</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 2500</v>
+        <v>, value: 2500</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-September, December-February (Northern) / November-March, June-August (Southern)"</v>
+        <v>, season: "April-September, December-February (Northern) / November-March, June-August (Southern)"</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" si="6"/>
@@ -1470,7 +1470,7 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 11, "name": "Raja Brooke's Birdwing", "type": "Flying by purple flowers", "value": 2500, "time": "8 a.m. - 5 p.m.", "season": "April-September, December-February (Northern) / November-March, June-August (Southern)" },</v>
+        <v>{ id: 11, name: "Raja Brooke's Birdwing", type: "Flying by purple flowers", value: 2500, time: "8 a.m. - 5 p.m.", season: "April-September, December-February (Northern) / November-March, June-August (Southern)" },</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -1494,27 +1494,27 @@
       </c>
       <c r="J15" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 12</v>
+        <v>{ id: 12</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Queen Alexandra's Birdwing"</v>
+        <v>, name: "Queen Alexandra's Birdwing"</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 4000</v>
+        <v>, value: 4000</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 4 p.m."</v>
+        <v>, time: "8 a.m. - 4 p.m."</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "May-September (Northern) / November-March (Southern)"</v>
+        <v>, season: "May-September (Northern) / November-March (Southern)"</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="6"/>
@@ -1523,7 +1523,7 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 12, "name": "Queen Alexandra's Birdwing", "type": "Flying", "value": 4000, "time": "8 a.m. - 4 p.m.", "season": "May-September (Northern) / November-March (Southern)" },</v>
+        <v>{ id: 12, name: "Queen Alexandra's Birdwing", type: "Flying", value: 4000, time: "8 a.m. - 4 p.m.", season: "May-September (Northern) / November-March (Southern)" },</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -1547,27 +1547,27 @@
       </c>
       <c r="J16" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 13</v>
+        <v>{ id: 13</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Moth"</v>
+        <v>, name: "Moth"</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying by light"</v>
+        <v>, type: "Flying by light"</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 130</v>
+        <v>, value: 130</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "7 p.m. - 4 a.m."</v>
+        <v>, time: "7 p.m. - 4 a.m."</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" si="6"/>
@@ -1576,7 +1576,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 13, "name": "Moth", "type": "Flying by light", "value": 130, "time": "7 p.m. - 4 a.m.", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 13, name: "Moth", type: "Flying by light", value: 130, time: "7 p.m. - 4 a.m.", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -1600,27 +1600,27 @@
       </c>
       <c r="J17" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 14</v>
+        <v>{ id: 14</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Atlas Moth"</v>
+        <v>, name: "Atlas Moth"</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M17" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 3000</v>
+        <v>, value: 3000</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "7 p.m. - 4 a.m."</v>
+        <v>, time: "7 p.m. - 4 a.m."</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-September (Northern) / October-March (Southern)"</v>
+        <v>, season: "April-September (Northern) / October-March (Southern)"</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" si="6"/>
@@ -1629,7 +1629,7 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 14, "name": "Atlas Moth", "type": "On trees", "value": 3000, "time": "7 p.m. - 4 a.m.", "season": "April-September (Northern) / October-March (Southern)" },</v>
+        <v>{ id: 14, name: "Atlas Moth", type: "On trees", value: 3000, time: "7 p.m. - 4 a.m.", season: "April-September (Northern) / October-March (Southern)" },</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -1653,27 +1653,27 @@
       </c>
       <c r="J18" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 15</v>
+        <v>{ id: 15</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Madagascan Sunset Moth"</v>
+        <v>, name: "Madagascan Sunset Moth"</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M18" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 2500</v>
+        <v>, value: 2500</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 4 p.m."</v>
+        <v>, time: "8 a.m. - 4 p.m."</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-September (Northern) / October-March (Southern)"</v>
+        <v>, season: "April-September (Northern) / October-March (Southern)"</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="6"/>
@@ -1682,7 +1682,7 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 15, "name": "Madagascan Sunset Moth", "type": "Flying", "value": 2500, "time": "8 a.m. - 4 p.m.", "season": "April-September (Northern) / October-March (Southern)" },</v>
+        <v>{ id: 15, name: "Madagascan Sunset Moth", type: "Flying", value: 2500, time: "8 a.m. - 4 p.m.", season: "April-September (Northern) / October-March (Southern)" },</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
@@ -1706,27 +1706,27 @@
       </c>
       <c r="J19" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 16</v>
+        <v>{ id: 16</v>
       </c>
       <c r="K19" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Long Locust"</v>
+        <v>, name: "Long Locust"</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M19" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 200</v>
+        <v>, value: 200</v>
       </c>
       <c r="N19" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 7 p.m."</v>
+        <v>, time: "8 a.m. - 7 p.m."</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-November (Northern) / November-May (Southern)"</v>
+        <v>, season: "April-November (Northern) / November-May (Southern)"</v>
       </c>
       <c r="P19" t="str">
         <f t="shared" si="6"/>
@@ -1735,7 +1735,7 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 16, "name": "Long Locust", "type": "On ground", "value": 200, "time": "8 a.m. - 7 p.m.", "season": "April-November (Northern) / November-May (Southern)" },</v>
+        <v>{ id: 16, name: "Long Locust", type: "On ground", value: 200, time: "8 a.m. - 7 p.m.", season: "April-November (Northern) / November-May (Southern)" },</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -1759,27 +1759,27 @@
       </c>
       <c r="J20" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 17</v>
+        <v>{ id: 17</v>
       </c>
       <c r="K20" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Migratory Locust"</v>
+        <v>, name: "Migratory Locust"</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M20" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 600</v>
+        <v>, value: 600</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 7 p.m."</v>
+        <v>, time: "8 a.m. - 7 p.m."</v>
       </c>
       <c r="O20" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "August-November (Northern) / February-May (Southern)"</v>
+        <v>, season: "August-November (Northern) / February-May (Southern)"</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" si="6"/>
@@ -1788,7 +1788,7 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 17, "name": "Migratory Locust", "type": "On ground", "value": 600, "time": "8 a.m. - 7 p.m.", "season": "August-November (Northern) / February-May (Southern)" },</v>
+        <v>{ id: 17, name: "Migratory Locust", type: "On ground", value: 600, time: "8 a.m. - 7 p.m.", season: "August-November (Northern) / February-May (Southern)" },</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
@@ -1812,27 +1812,27 @@
       </c>
       <c r="J21" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 18</v>
+        <v>{ id: 18</v>
       </c>
       <c r="K21" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Rice Grasshopper"</v>
+        <v>, name: "Rice Grasshopper"</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M21" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 160</v>
+        <v>, value: 160</v>
       </c>
       <c r="N21" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 7 p.m."</v>
+        <v>, time: "8 a.m. - 7 p.m."</v>
       </c>
       <c r="O21" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "August-November (Northern) / February-May (Southern)"</v>
+        <v>, season: "August-November (Northern) / February-May (Southern)"</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" si="6"/>
@@ -1841,7 +1841,7 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 18, "name": "Rice Grasshopper", "type": "On ground", "value": 160, "time": "8 a.m. - 7 p.m.", "season": "August-November (Northern) / February-May (Southern)" },</v>
+        <v>{ id: 18, name: "Rice Grasshopper", type: "On ground", value: 160, time: "8 a.m. - 7 p.m.", season: "August-November (Northern) / February-May (Southern)" },</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
@@ -1865,27 +1865,27 @@
       </c>
       <c r="J22" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 19</v>
+        <v>{ id: 19</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Grasshopper"</v>
+        <v>, name: "Grasshopper"</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M22" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 160</v>
+        <v>, value: 160</v>
       </c>
       <c r="N22" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O22" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-September (Northern) / January-March (Southern)"</v>
+        <v>, season: "July-September (Northern) / January-March (Southern)"</v>
       </c>
       <c r="P22" t="str">
         <f t="shared" si="6"/>
@@ -1894,7 +1894,7 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 19, "name": "Grasshopper", "type": "On ground", "value": 160, "time": "8 a.m. - 5 p.m.", "season": "July-September (Northern) / January-March (Southern)" },</v>
+        <v>{ id: 19, name: "Grasshopper", type: "On ground", value: 160, time: "8 a.m. - 5 p.m.", season: "July-September (Northern) / January-March (Southern)" },</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -1918,27 +1918,27 @@
       </c>
       <c r="J23" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 20</v>
+        <v>{ id: 20</v>
       </c>
       <c r="K23" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Cricket"</v>
+        <v>, name: "Cricket"</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M23" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 130</v>
+        <v>, value: 130</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "September-November (Northern) / March-May (Southern)"</v>
+        <v>, season: "September-November (Northern) / March-May (Southern)"</v>
       </c>
       <c r="P23" t="str">
         <f t="shared" si="6"/>
@@ -1947,7 +1947,7 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 20, "name": "Cricket", "type": "On ground", "value": 130, "time": "5 p.m. - 8 a.m.", "season": "September-November (Northern) / March-May (Southern)" },</v>
+        <v>{ id: 20, name: "Cricket", type: "On ground", value: 130, time: "5 p.m. - 8 a.m.", season: "September-November (Northern) / March-May (Southern)" },</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
@@ -1971,27 +1971,27 @@
       </c>
       <c r="J24" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 21</v>
+        <v>{ id: 21</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Bell Cricket"</v>
+        <v>, name: "Bell Cricket"</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M24" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 430</v>
+        <v>, value: 430</v>
       </c>
       <c r="N24" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "September-October (Northern) / March-April (Southern)"</v>
+        <v>, season: "September-October (Northern) / March-April (Southern)"</v>
       </c>
       <c r="P24" t="str">
         <f t="shared" si="6"/>
@@ -2000,7 +2000,7 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 21, "name": "Bell Cricket", "type": "On ground", "value": 430, "time": "5 p.m. - 8 a.m.", "season": "September-October (Northern) / March-April (Southern)" },</v>
+        <v>{ id: 21, name: "Bell Cricket", type: "On ground", value: 430, time: "5 p.m. - 8 a.m.", season: "September-October (Northern) / March-April (Southern)" },</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
@@ -2024,27 +2024,27 @@
       </c>
       <c r="J25" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 22</v>
+        <v>{ id: 22</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Mantis"</v>
+        <v>, name: "Mantis"</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On flowers"</v>
+        <v>, type: "On flowers"</v>
       </c>
       <c r="M25" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 430</v>
+        <v>, value: 430</v>
       </c>
       <c r="N25" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "March-November (Northern) / September-May (Southern)"</v>
+        <v>, season: "March-November (Northern) / September-May (Southern)"</v>
       </c>
       <c r="P25" t="str">
         <f t="shared" si="6"/>
@@ -2053,7 +2053,7 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 22, "name": "Mantis", "type": "On flowers", "value": 430, "time": "8 a.m. - 5 p.m.", "season": "March-November (Northern) / September-May (Southern)" },</v>
+        <v>{ id: 22, name: "Mantis", type: "On flowers", value: 430, time: "8 a.m. - 5 p.m.", season: "March-November (Northern) / September-May (Southern)" },</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
@@ -2077,27 +2077,27 @@
       </c>
       <c r="J26" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 23</v>
+        <v>{ id: 23</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Orchid Mantis"</v>
+        <v>, name: "Orchid Mantis"</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On white flowers"</v>
+        <v>, type: "On white flowers"</v>
       </c>
       <c r="M26" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 2400</v>
+        <v>, value: 2400</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "March-November (Northern) / September-May (Southern)"</v>
+        <v>, season: "March-November (Northern) / September-May (Southern)"</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" si="6"/>
@@ -2106,7 +2106,7 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 23, "name": "Orchid Mantis", "type": "On white flowers", "value": 2400, "time": "8 a.m. - 5 p.m.", "season": "March-November (Northern) / September-May (Southern)" },</v>
+        <v>{ id: 23, name: "Orchid Mantis", type: "On white flowers", value: 2400, time: "8 a.m. - 5 p.m.", season: "March-November (Northern) / September-May (Southern)" },</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
@@ -2130,27 +2130,27 @@
       </c>
       <c r="J27" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 24</v>
+        <v>{ id: 24</v>
       </c>
       <c r="K27" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Honeybee"</v>
+        <v>, name: "Honeybee"</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M27" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 200</v>
+        <v>, value: 200</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "March-July (Northern) / March-July (Southern)"</v>
+        <v>, season: "March-July (Northern) / March-July (Southern)"</v>
       </c>
       <c r="P27" t="str">
         <f t="shared" si="6"/>
@@ -2159,7 +2159,7 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 24, "name": "Honeybee", "type": "Flying", "value": 200, "time": "8 a.m. - 5 p.m.", "season": "March-July (Northern) / March-July (Southern)" },</v>
+        <v>{ id: 24, name: "Honeybee", type: "Flying", value: 200, time: "8 a.m. - 5 p.m.", season: "March-July (Northern) / March-July (Southern)" },</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
@@ -2183,27 +2183,27 @@
       </c>
       <c r="J28" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 25</v>
+        <v>{ id: 25</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Wasp"</v>
+        <v>, name: "Wasp"</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Falls from shaking trees"</v>
+        <v>, type: "Falls from shaking trees"</v>
       </c>
       <c r="M28" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 2500</v>
+        <v>, value: 2500</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P28" t="str">
         <f t="shared" si="6"/>
@@ -2212,7 +2212,7 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 25, "name": "Wasp", "type": "Falls from shaking trees", "value": 2500, "time": "All day", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 25, name: "Wasp", type: "Falls from shaking trees", value: 2500, time: "All day", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -2236,27 +2236,27 @@
       </c>
       <c r="J29" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 26</v>
+        <v>{ id: 26</v>
       </c>
       <c r="K29" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Brown Cicada"</v>
+        <v>, name: "Brown Cicada"</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M29" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 250</v>
+        <v>, value: 250</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P29" t="str">
         <f t="shared" si="6"/>
@@ -2265,7 +2265,7 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 26, "name": "Brown Cicada", "type": "On trees", "value": 250, "time": "8 a.m. - 5 p.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 26, name: "Brown Cicada", type: "On trees", value: 250, time: "8 a.m. - 5 p.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
@@ -2289,27 +2289,27 @@
       </c>
       <c r="J30" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 27</v>
+        <v>{ id: 27</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Robust Cicada"</v>
+        <v>, name: "Robust Cicada"</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M30" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 300</v>
+        <v>, value: 300</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P30" t="str">
         <f t="shared" si="6"/>
@@ -2318,7 +2318,7 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 27, "name": "Robust Cicada", "type": "On trees", "value": 300, "time": "8 a.m. - 5 p.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 27, name: "Robust Cicada", type: "On trees", value: 300, time: "8 a.m. - 5 p.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
@@ -2342,27 +2342,27 @@
       </c>
       <c r="J31" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 28</v>
+        <v>{ id: 28</v>
       </c>
       <c r="K31" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Giant Cicada"</v>
+        <v>, name: "Giant Cicada"</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 600</v>
+        <v>, value: 600</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P31" t="str">
         <f t="shared" si="6"/>
@@ -2371,7 +2371,7 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 28, "name": "Giant Cicada", "type": "On trees", "value": 600, "time": "8 a.m. - 5 p.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 28, name: "Giant Cicada", type: "On trees", value: 600, time: "8 a.m. - 5 p.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
@@ -2395,27 +2395,27 @@
       </c>
       <c r="J32" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 29</v>
+        <v>{ id: 29</v>
       </c>
       <c r="K32" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Walker Cicada"</v>
+        <v>, name: "Walker Cicada"</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 400</v>
+        <v>, value: 400</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "August-September (Northern) / February-March (Southern)"</v>
+        <v>, season: "August-September (Northern) / February-March (Southern)"</v>
       </c>
       <c r="P32" t="str">
         <f t="shared" si="6"/>
@@ -2424,7 +2424,7 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 29, "name": "Walker Cicada", "type": "On trees", "value": 400, "time": "8 a.m. - 5 p.m.", "season": "August-September (Northern) / February-March (Southern)" },</v>
+        <v>{ id: 29, name: "Walker Cicada", type: "On trees", value: 400, time: "8 a.m. - 5 p.m.", season: "August-September (Northern) / February-March (Southern)" },</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
@@ -2448,27 +2448,27 @@
       </c>
       <c r="J33" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 30</v>
+        <v>{ id: 30</v>
       </c>
       <c r="K33" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Evening Cicada"</v>
+        <v>, name: "Evening Cicada"</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 660</v>
+        <v>, value: 660</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "4 a.m. - 8 a.m., 4 p.m. - 7 p.m."</v>
+        <v>, time: "4 a.m. - 8 a.m., 4 p.m. - 7 p.m."</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P33" t="str">
         <f t="shared" si="6"/>
@@ -2477,7 +2477,7 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 30, "name": "Evening Cicada", "type": "On trees", "value": 660, "time": "4 a.m. - 8 a.m., 4 p.m. - 7 p.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 30, name: "Evening Cicada", type: "On trees", value: 660, time: "4 a.m. - 8 a.m., 4 p.m. - 7 p.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
@@ -2501,27 +2501,27 @@
       </c>
       <c r="J34" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 31</v>
+        <v>{ id: 31</v>
       </c>
       <c r="K34" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Cicada Shell"</v>
+        <v>, name: "Cicada Shell"</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 10</v>
+        <v>, value: 10</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P34" t="str">
         <f t="shared" si="6"/>
@@ -2530,7 +2530,7 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 31, "name": "Cicada Shell", "type": "On trees", "value": 10, "time": "All day", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 31, name: "Cicada Shell", type: "On trees", value: 10, time: "All day", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -2554,27 +2554,27 @@
       </c>
       <c r="J35" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 32</v>
+        <v>{ id: 32</v>
       </c>
       <c r="K35" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Red Dragonfly"</v>
+        <v>, name: "Red Dragonfly"</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 180</v>
+        <v>, value: 180</v>
       </c>
       <c r="N35" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 7 p.m."</v>
+        <v>, time: "8 a.m. - 7 p.m."</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "September-October (Northern) / March-April (Southern)"</v>
+        <v>, season: "September-October (Northern) / March-April (Southern)"</v>
       </c>
       <c r="P35" t="str">
         <f t="shared" si="6"/>
@@ -2583,7 +2583,7 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 32, "name": "Red Dragonfly", "type": "Flying", "value": 180, "time": "8 a.m. - 7 p.m.", "season": "September-October (Northern) / March-April (Southern)" },</v>
+        <v>{ id: 32, name: "Red Dragonfly", type: "Flying", value: 180, time: "8 a.m. - 7 p.m.", season: "September-October (Northern) / March-April (Southern)" },</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
@@ -2607,27 +2607,27 @@
       </c>
       <c r="J36" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 33</v>
+        <v>{ id: 33</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Darner Dragonfly"</v>
+        <v>, name: "Darner Dragonfly"</v>
       </c>
       <c r="L36" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M36" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 230</v>
+        <v>, value: 230</v>
       </c>
       <c r="N36" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O36" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-October (Northern) / October-April (Southern)"</v>
+        <v>, season: "April-October (Northern) / October-April (Southern)"</v>
       </c>
       <c r="P36" t="str">
         <f t="shared" si="6"/>
@@ -2636,7 +2636,7 @@
       <c r="Q36" s="2"/>
       <c r="R36" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 33, "name": "Darner Dragonfly", "type": "Flying", "value": 230, "time": "8 a.m. - 5 p.m.", "season": "April-October (Northern) / October-April (Southern)" },</v>
+        <v>{ id: 33, name: "Darner Dragonfly", type: "Flying", value: 230, time: "8 a.m. - 5 p.m.", season: "April-October (Northern) / October-April (Southern)" },</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
@@ -2660,27 +2660,27 @@
       </c>
       <c r="J37" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 34</v>
+        <v>{ id: 34</v>
       </c>
       <c r="K37" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Banded Dragonfly"</v>
+        <v>, name: "Banded Dragonfly"</v>
       </c>
       <c r="L37" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M37" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 4500</v>
+        <v>, value: 4500</v>
       </c>
       <c r="N37" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O37" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "May-October (Northern) / November-April (Southern)"</v>
+        <v>, season: "May-October (Northern) / November-April (Southern)"</v>
       </c>
       <c r="P37" t="str">
         <f t="shared" si="6"/>
@@ -2689,7 +2689,7 @@
       <c r="Q37" s="2"/>
       <c r="R37" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 34, "name": "Banded Dragonfly", "type": "Flying", "value": 4500, "time": "8 a.m. - 5 p.m.", "season": "May-October (Northern) / November-April (Southern)" },</v>
+        <v>{ id: 34, name: "Banded Dragonfly", type: "Flying", value: 4500, time: "8 a.m. - 5 p.m.", season: "May-October (Northern) / November-April (Southern)" },</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
@@ -2713,27 +2713,27 @@
       </c>
       <c r="J38" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 35</v>
+        <v>{ id: 35</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Damselfly"</v>
+        <v>, name: "Damselfly"</v>
       </c>
       <c r="L38" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M38" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 500</v>
+        <v>, value: 500</v>
       </c>
       <c r="N38" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O38" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "November-February (Northern) / May-August (Southern)"</v>
+        <v>, season: "November-February (Northern) / May-August (Southern)"</v>
       </c>
       <c r="P38" t="str">
         <f t="shared" si="6"/>
@@ -2742,7 +2742,7 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 35, "name": "Damselfly", "type": "Flying", "value": 500, "time": "All day", "season": "November-February (Northern) / May-August (Southern)" },</v>
+        <v>{ id: 35, name: "Damselfly", type: "Flying", value: 500, time: "All day", season: "November-February (Northern) / May-August (Southern)" },</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
@@ -2766,27 +2766,27 @@
       </c>
       <c r="J39" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 36</v>
+        <v>{ id: 36</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Firefly"</v>
+        <v>, name: "Firefly"</v>
       </c>
       <c r="L39" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M39" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 300</v>
+        <v>, value: 300</v>
       </c>
       <c r="N39" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "7 p.m. - 4 a.m."</v>
+        <v>, time: "7 p.m. - 4 a.m."</v>
       </c>
       <c r="O39" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "June (Northern) / December (Southern)"</v>
+        <v>, season: "June (Northern) / December (Southern)"</v>
       </c>
       <c r="P39" t="str">
         <f t="shared" si="6"/>
@@ -2795,7 +2795,7 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 36, "name": "Firefly", "type": "Flying", "value": 300, "time": "7 p.m. - 4 a.m.", "season": "June (Northern) / December (Southern)" },</v>
+        <v>{ id: 36, name: "Firefly", type: "Flying", value: 300, time: "7 p.m. - 4 a.m.", season: "June (Northern) / December (Southern)" },</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
@@ -2819,27 +2819,27 @@
       </c>
       <c r="J40" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 37</v>
+        <v>{ id: 37</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Mole Cricket"</v>
+        <v>, name: "Mole Cricket"</v>
       </c>
       <c r="L40" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Underground"</v>
+        <v>, type: "Underground"</v>
       </c>
       <c r="M40" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 500</v>
+        <v>, value: 500</v>
       </c>
       <c r="N40" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O40" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "November-May (Northern) / May-November (Southern)"</v>
+        <v>, season: "November-May (Northern) / May-November (Southern)"</v>
       </c>
       <c r="P40" t="str">
         <f t="shared" si="6"/>
@@ -2848,7 +2848,7 @@
       <c r="Q40" s="2"/>
       <c r="R40" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 37, "name": "Mole Cricket", "type": "Underground", "value": 500, "time": "All day", "season": "November-May (Northern) / May-November (Southern)" },</v>
+        <v>{ id: 37, name: "Mole Cricket", type: "Underground", value: 500, time: "All day", season: "November-May (Northern) / May-November (Southern)" },</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
@@ -2872,27 +2872,27 @@
       </c>
       <c r="J41" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 38</v>
+        <v>{ id: 38</v>
       </c>
       <c r="K41" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Pondskater"</v>
+        <v>, name: "Pondskater"</v>
       </c>
       <c r="L41" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Ponds"</v>
+        <v>, type: "Ponds"</v>
       </c>
       <c r="M41" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 130</v>
+        <v>, value: 130</v>
       </c>
       <c r="N41" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 7 p.m."</v>
+        <v>, time: "8 a.m. - 7 p.m."</v>
       </c>
       <c r="O41" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "May-September (Northern) / November-March (Southern)"</v>
+        <v>, season: "May-September (Northern) / November-March (Southern)"</v>
       </c>
       <c r="P41" t="str">
         <f t="shared" si="6"/>
@@ -2901,7 +2901,7 @@
       <c r="Q41" s="2"/>
       <c r="R41" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 38, "name": "Pondskater", "type": "Ponds", "value": 130, "time": "8 a.m. - 7 p.m.", "season": "May-September (Northern) / November-March (Southern)" },</v>
+        <v>{ id: 38, name: "Pondskater", type: "Ponds", value: 130, time: "8 a.m. - 7 p.m.", season: "May-September (Northern) / November-March (Southern)" },</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -2925,27 +2925,27 @@
       </c>
       <c r="J42" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 39</v>
+        <v>{ id: 39</v>
       </c>
       <c r="K42" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Diving Beetle"</v>
+        <v>, name: "Diving Beetle"</v>
       </c>
       <c r="L42" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Ponds and rivers"</v>
+        <v>, type: "Ponds and rivers"</v>
       </c>
       <c r="M42" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 800</v>
+        <v>, value: 800</v>
       </c>
       <c r="N42" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 7 p.m."</v>
+        <v>, time: "8 a.m. - 7 p.m."</v>
       </c>
       <c r="O42" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "May-September (Northern) / November-March (Southern)"</v>
+        <v>, season: "May-September (Northern) / November-March (Southern)"</v>
       </c>
       <c r="P42" t="str">
         <f t="shared" si="6"/>
@@ -2954,7 +2954,7 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 39, "name": "Diving Beetle", "type": "Ponds and rivers", "value": 800, "time": "8 a.m. - 7 p.m.", "season": "May-September (Northern) / November-March (Southern)" },</v>
+        <v>{ id: 39, name: "Diving Beetle", type: "Ponds and rivers", value: 800, time: "8 a.m. - 7 p.m.", season: "May-September (Northern) / November-March (Southern)" },</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
@@ -2978,27 +2978,27 @@
       </c>
       <c r="J43" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 40</v>
+        <v>{ id: 40</v>
       </c>
       <c r="K43" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Giant Water Bug"</v>
+        <v>, name: "Giant Water Bug"</v>
       </c>
       <c r="L43" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Ponds and rivers"</v>
+        <v>, type: "Ponds and rivers"</v>
       </c>
       <c r="M43" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 2000</v>
+        <v>, value: 2000</v>
       </c>
       <c r="N43" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "7 p.m. - 8 a.m."</v>
+        <v>, time: "7 p.m. - 8 a.m."</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-September (Northern) / October-March (Southern)"</v>
+        <v>, season: "April-September (Northern) / October-March (Southern)"</v>
       </c>
       <c r="P43" t="str">
         <f t="shared" si="6"/>
@@ -3007,7 +3007,7 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 40, "name": "Giant Water Bug", "type": "Ponds and rivers", "value": 2000, "time": "7 p.m. - 8 a.m.", "season": "April-September (Northern) / October-March (Southern)" },</v>
+        <v>{ id: 40, name: "Giant Water Bug", type: "Ponds and rivers", value: 2000, time: "7 p.m. - 8 a.m.", season: "April-September (Northern) / October-March (Southern)" },</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -3031,27 +3031,27 @@
       </c>
       <c r="J44" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 41</v>
+        <v>{ id: 41</v>
       </c>
       <c r="K44" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Stinkbug"</v>
+        <v>, name: "Stinkbug"</v>
       </c>
       <c r="L44" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On flowers"</v>
+        <v>, type: "On flowers"</v>
       </c>
       <c r="M44" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 120</v>
+        <v>, value: 120</v>
       </c>
       <c r="N44" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "March-November (Northern) / September-May (Southern)"</v>
+        <v>, season: "March-November (Northern) / September-May (Southern)"</v>
       </c>
       <c r="P44" t="str">
         <f t="shared" si="6"/>
@@ -3060,7 +3060,7 @@
       <c r="Q44" s="2"/>
       <c r="R44" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 41, "name": "Stinkbug", "type": "On flowers", "value": 120, "time": "All day", "season": "March-November (Northern) / September-May (Southern)" },</v>
+        <v>{ id: 41, name: "Stinkbug", type: "On flowers", value: 120, time: "All day", season: "March-November (Northern) / September-May (Southern)" },</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -3084,27 +3084,27 @@
       </c>
       <c r="J45" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 42</v>
+        <v>{ id: 42</v>
       </c>
       <c r="K45" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Man-faced Stink Bug"</v>
+        <v>, name: "Man-faced Stink Bug"</v>
       </c>
       <c r="L45" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On flowers"</v>
+        <v>, type: "On flowers"</v>
       </c>
       <c r="M45" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 1000</v>
+        <v>, value: 1000</v>
       </c>
       <c r="N45" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "7 p.m. - 8 a.m."</v>
+        <v>, time: "7 p.m. - 8 a.m."</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "March-November (Northern) / September-May (Southern)"</v>
+        <v>, season: "March-November (Northern) / September-May (Southern)"</v>
       </c>
       <c r="P45" t="str">
         <f t="shared" si="6"/>
@@ -3113,7 +3113,7 @@
       <c r="Q45" s="2"/>
       <c r="R45" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 42, "name": "Man-faced Stink Bug", "type": "On flowers", "value": 1000, "time": "7 p.m. - 8 a.m.", "season": "March-November (Northern) / September-May (Southern)" },</v>
+        <v>{ id: 42, name: "Man-faced Stink Bug", type: "On flowers", value: 1000, time: "7 p.m. - 8 a.m.", season: "March-November (Northern) / September-May (Southern)" },</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
@@ -3137,27 +3137,27 @@
       </c>
       <c r="J46" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 43</v>
+        <v>{ id: 43</v>
       </c>
       <c r="K46" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Ladybug"</v>
+        <v>, name: "Ladybug"</v>
       </c>
       <c r="L46" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On flowers"</v>
+        <v>, type: "On flowers"</v>
       </c>
       <c r="M46" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 200</v>
+        <v>, value: 200</v>
       </c>
       <c r="N46" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "8 a.m. - 5 p.m."</v>
+        <v>, time: "8 a.m. - 5 p.m."</v>
       </c>
       <c r="O46" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "March-June, October (Northern) / September-December, April (Southern)"</v>
+        <v>, season: "March-June, October (Northern) / September-December, April (Southern)"</v>
       </c>
       <c r="P46" t="str">
         <f t="shared" si="6"/>
@@ -3166,7 +3166,7 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 43, "name": "Ladybug", "type": "On flowers", "value": 200, "time": "8 a.m. - 5 p.m.", "season": "March-June, October (Northern) / September-December, April (Southern)" },</v>
+        <v>{ id: 43, name: "Ladybug", type: "On flowers", value: 200, time: "8 a.m. - 5 p.m.", season: "March-June, October (Northern) / September-December, April (Southern)" },</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
@@ -3190,27 +3190,27 @@
       </c>
       <c r="J47" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 44</v>
+        <v>{ id: 44</v>
       </c>
       <c r="K47" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Tiger Beetle"</v>
+        <v>, name: "Tiger Beetle"</v>
       </c>
       <c r="L47" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M47" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 1500</v>
+        <v>, value: 1500</v>
       </c>
       <c r="N47" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O47" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "February-November (Northern) / August-May (Southern)"</v>
+        <v>, season: "February-November (Northern) / August-May (Southern)"</v>
       </c>
       <c r="P47" t="str">
         <f t="shared" si="6"/>
@@ -3219,7 +3219,7 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 44, "name": "Tiger Beetle", "type": "On ground", "value": 1500, "time": "All day", "season": "February-November (Northern) / August-May (Southern)" },</v>
+        <v>{ id: 44, name: "Tiger Beetle", type: "On ground", value: 1500, time: "All day", season: "February-November (Northern) / August-May (Southern)" },</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
@@ -3243,27 +3243,27 @@
       </c>
       <c r="J48" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 45</v>
+        <v>{ id: 45</v>
       </c>
       <c r="K48" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Jewel Beetle"</v>
+        <v>, name: "Jewel Beetle"</v>
       </c>
       <c r="L48" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On tree stumps"</v>
+        <v>, type: "On tree stumps"</v>
       </c>
       <c r="M48" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 2400</v>
+        <v>, value: 2400</v>
       </c>
       <c r="N48" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "April-August (Northern) / October-February (Southern)"</v>
+        <v>, season: "April-August (Northern) / October-February (Southern)"</v>
       </c>
       <c r="P48" t="str">
         <f t="shared" si="6"/>
@@ -3272,7 +3272,7 @@
       <c r="Q48" s="2"/>
       <c r="R48" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 45, "name": "Jewel Beetle", "type": "On tree stumps", "value": 2400, "time": "All day", "season": "April-August (Northern) / October-February (Southern)" },</v>
+        <v>{ id: 45, name: "Jewel Beetle", type: "On tree stumps", value: 2400, time: "All day", season: "April-August (Northern) / October-February (Southern)" },</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -3296,27 +3296,27 @@
       </c>
       <c r="J49" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 46</v>
+        <v>{ id: 46</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Violin Beetle"</v>
+        <v>, name: "Violin Beetle"</v>
       </c>
       <c r="L49" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On tree stumps"</v>
+        <v>, type: "On tree stumps"</v>
       </c>
       <c r="M49" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 450</v>
+        <v>, value: 450</v>
       </c>
       <c r="N49" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O49" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "May-June, September-November (Northern) / November-December, March-April (Southern)"</v>
+        <v>, season: "May-June, September-November (Northern) / November-December, March-April (Southern)"</v>
       </c>
       <c r="P49" t="str">
         <f t="shared" si="6"/>
@@ -3325,7 +3325,7 @@
       <c r="Q49" s="2"/>
       <c r="R49" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 46, "name": "Violin Beetle", "type": "On tree stumps", "value": 450, "time": "All day", "season": "May-June, September-November (Northern) / November-December, March-April (Southern)" },</v>
+        <v>{ id: 46, name: "Violin Beetle", type: "On tree stumps", value: 450, time: "All day", season: "May-June, September-November (Northern) / November-December, March-April (Southern)" },</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
@@ -3349,27 +3349,27 @@
       </c>
       <c r="J50" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 47</v>
+        <v>{ id: 47</v>
       </c>
       <c r="K50" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Citrus Long-horned Beetle"</v>
+        <v>, name: "Citrus Long-horned Beetle"</v>
       </c>
       <c r="L50" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On tree stumps"</v>
+        <v>, type: "On tree stumps"</v>
       </c>
       <c r="M50" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 350</v>
+        <v>, value: 350</v>
       </c>
       <c r="N50" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O50" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P50" t="str">
         <f t="shared" si="6"/>
@@ -3378,7 +3378,7 @@
       <c r="Q50" s="2"/>
       <c r="R50" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 47, "name": "Citrus Long-horned Beetle", "type": "On tree stumps", "value": 350, "time": "All day", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 47, name: "Citrus Long-horned Beetle", type: "On tree stumps", value: 350, time: "All day", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
@@ -3402,27 +3402,27 @@
       </c>
       <c r="J51" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 48</v>
+        <v>{ id: 48</v>
       </c>
       <c r="K51" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Rosalia Batesi Beetle"</v>
+        <v>, name: "Rosalia Batesi Beetle"</v>
       </c>
       <c r="L51" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On tree stumps"</v>
+        <v>, type: "On tree stumps"</v>
       </c>
       <c r="M51" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 3000</v>
+        <v>, value: 3000</v>
       </c>
       <c r="N51" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O51" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "May-September (Northern) / November-March (Southern)"</v>
+        <v>, season: "May-September (Northern) / November-March (Southern)"</v>
       </c>
       <c r="P51" t="str">
         <f t="shared" si="6"/>
@@ -3431,7 +3431,7 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 48, "name": "Rosalia Batesi Beetle", "type": "On tree stumps", "value": 3000, "time": "All day", "season": "May-September (Northern) / November-March (Southern)" },</v>
+        <v>{ id: 48, name: "Rosalia Batesi Beetle", type: "On tree stumps", value: 3000, time: "All day", season: "May-September (Northern) / November-March (Southern)" },</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
@@ -3455,27 +3455,27 @@
       </c>
       <c r="J52" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 49</v>
+        <v>{ id: 49</v>
       </c>
       <c r="K52" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Blue Weevil Beetle"</v>
+        <v>, name: "Blue Weevil Beetle"</v>
       </c>
       <c r="L52" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On coconut trees"</v>
+        <v>, type: "On coconut trees"</v>
       </c>
       <c r="M52" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 800</v>
+        <v>, value: 800</v>
       </c>
       <c r="N52" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O52" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P52" t="str">
         <f t="shared" si="6"/>
@@ -3484,7 +3484,7 @@
       <c r="Q52" s="2"/>
       <c r="R52" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 49, "name": "Blue Weevil Beetle", "type": "On coconut trees", "value": 800, "time": "All day", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 49, name: "Blue Weevil Beetle", type: "On coconut trees", value: 800, time: "All day", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
@@ -3505,27 +3505,27 @@
       </c>
       <c r="J53" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 50</v>
+        <v>{ id: 50</v>
       </c>
       <c r="K53" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Dung Beetle"</v>
+        <v>, name: "Dung Beetle"</v>
       </c>
       <c r="L53" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "Pushing snowballs"</v>
+        <v>, type: "Pushing snowballs"</v>
       </c>
       <c r="M53" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 3000</v>
+        <v>, value: 3000</v>
       </c>
       <c r="N53" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": ""</v>
+        <v>, time: ""</v>
       </c>
       <c r="O53" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "December-February (Northern) / June-August (Southern)"</v>
+        <v>, season: "December-February (Northern) / June-August (Southern)"</v>
       </c>
       <c r="P53" t="str">
         <f t="shared" si="6"/>
@@ -3534,7 +3534,7 @@
       <c r="Q53" s="2"/>
       <c r="R53" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 50, "name": "Dung Beetle", "type": "Pushing snowballs", "value": 3000, "time": "", "season": "December-February (Northern) / June-August (Southern)" },</v>
+        <v>{ id: 50, name: "Dung Beetle", type: "Pushing snowballs", value: 3000, time: "", season: "December-February (Northern) / June-August (Southern)" },</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
@@ -3558,27 +3558,27 @@
       </c>
       <c r="J54" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 51</v>
+        <v>{ id: 51</v>
       </c>
       <c r="K54" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Earth-boring Dung Beetle"</v>
+        <v>, name: "Earth-boring Dung Beetle"</v>
       </c>
       <c r="L54" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M54" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 300</v>
+        <v>, value: 300</v>
       </c>
       <c r="N54" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O54" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-September (Northern) / January-March (Southern)"</v>
+        <v>, season: "July-September (Northern) / January-March (Southern)"</v>
       </c>
       <c r="P54" t="str">
         <f t="shared" si="6"/>
@@ -3587,7 +3587,7 @@
       <c r="Q54" s="2"/>
       <c r="R54" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 51, "name": "Earth-boring Dung Beetle", "type": "On ground", "value": 300, "time": "All day", "season": "July-September (Northern) / January-March (Southern)" },</v>
+        <v>{ id: 51, name: "Earth-boring Dung Beetle", type: "On ground", value: 300, time: "All day", season: "July-September (Northern) / January-March (Southern)" },</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
@@ -3611,27 +3611,27 @@
       </c>
       <c r="J55" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 52</v>
+        <v>{ id: 52</v>
       </c>
       <c r="K55" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Scarab Beetle"</v>
+        <v>, name: "Scarab Beetle"</v>
       </c>
       <c r="L55" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M55" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 10000</v>
+        <v>, value: 10000</v>
       </c>
       <c r="N55" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "11 p.m. - 8 a.m."</v>
+        <v>, time: "11 p.m. - 8 a.m."</v>
       </c>
       <c r="O55" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P55" t="str">
         <f t="shared" si="6"/>
@@ -3640,7 +3640,7 @@
       <c r="Q55" s="2"/>
       <c r="R55" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 52, "name": "Scarab Beetle", "type": "On trees", "value": 10000, "time": "11 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 52, name: "Scarab Beetle", type: "On trees", value: 10000, time: "11 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
@@ -3664,27 +3664,27 @@
       </c>
       <c r="J56" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 53</v>
+        <v>{ id: 53</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Drone Beetle"</v>
+        <v>, name: "Drone Beetle"</v>
       </c>
       <c r="L56" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M56" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 200</v>
+        <v>, value: 200</v>
       </c>
       <c r="N56" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O56" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "June-August (Northern) / December-February (Southern)"</v>
+        <v>, season: "June-August (Northern) / December-February (Southern)"</v>
       </c>
       <c r="P56" t="str">
         <f t="shared" si="6"/>
@@ -3693,7 +3693,7 @@
       <c r="Q56" s="2"/>
       <c r="R56" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 53, "name": "Drone Beetle", "type": "On trees", "value": 200, "time": "All day", "season": "June-August (Northern) / December-February (Southern)" },</v>
+        <v>{ id: 53, name: "Drone Beetle", type: "On trees", value: 200, time: "All day", season: "June-August (Northern) / December-February (Southern)" },</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
@@ -3717,27 +3717,27 @@
       </c>
       <c r="J57" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 54</v>
+        <v>{ id: 54</v>
       </c>
       <c r="K57" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Goliath Beetle"</v>
+        <v>, name: "Goliath Beetle"</v>
       </c>
       <c r="L57" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On coconut trees"</v>
+        <v>, type: "On coconut trees"</v>
       </c>
       <c r="M57" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 8000</v>
+        <v>, value: 8000</v>
       </c>
       <c r="N57" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O57" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "June-September (Northern) / December-March (Southern)"</v>
+        <v>, season: "June-September (Northern) / December-March (Southern)"</v>
       </c>
       <c r="P57" t="str">
         <f t="shared" si="6"/>
@@ -3746,7 +3746,7 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 54, "name": "Goliath Beetle", "type": "On coconut trees", "value": 8000, "time": "5 p.m. - 8 a.m.", "season": "June-September (Northern) / December-March (Southern)" },</v>
+        <v>{ id: 54, name: "Goliath Beetle", type: "On coconut trees", value: 8000, time: "5 p.m. - 8 a.m.", season: "June-September (Northern) / December-March (Southern)" },</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
@@ -3770,27 +3770,27 @@
       </c>
       <c r="J58" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 55</v>
+        <v>{ id: 55</v>
       </c>
       <c r="K58" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Saw Stag"</v>
+        <v>, name: "Saw Stag"</v>
       </c>
       <c r="L58" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M58" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 2000</v>
+        <v>, value: 2000</v>
       </c>
       <c r="N58" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O58" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P58" t="str">
         <f t="shared" si="6"/>
@@ -3799,7 +3799,7 @@
       <c r="Q58" s="2"/>
       <c r="R58" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 55, "name": "Saw Stag", "type": "On trees", "value": 2000, "time": "All day", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 55, name: "Saw Stag", type: "On trees", value: 2000, time: "All day", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -3823,27 +3823,27 @@
       </c>
       <c r="J59" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 56</v>
+        <v>{ id: 56</v>
       </c>
       <c r="K59" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Miyama Stag"</v>
+        <v>, name: "Miyama Stag"</v>
       </c>
       <c r="L59" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M59" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 1000</v>
+        <v>, value: 1000</v>
       </c>
       <c r="N59" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O59" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P59" t="str">
         <f t="shared" si="6"/>
@@ -3852,7 +3852,7 @@
       <c r="Q59" s="2"/>
       <c r="R59" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 56, "name": "Miyama Stag", "type": "On trees", "value": 1000, "time": "All day", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 56, name: "Miyama Stag", type: "On trees", value: 1000, time: "All day", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
@@ -3876,27 +3876,27 @@
       </c>
       <c r="J60" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 57</v>
+        <v>{ id: 57</v>
       </c>
       <c r="K60" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Giant Stag"</v>
+        <v>, name: "Giant Stag"</v>
       </c>
       <c r="L60" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M60" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 10000</v>
+        <v>, value: 10000</v>
       </c>
       <c r="N60" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "11 p.m. - 8 a.m."</v>
+        <v>, time: "11 p.m. - 8 a.m."</v>
       </c>
       <c r="O60" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P60" t="str">
         <f t="shared" si="6"/>
@@ -3905,7 +3905,7 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 57, "name": "Giant Stag", "type": "On trees", "value": 10000, "time": "11 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 57, name: "Giant Stag", type: "On trees", value: 10000, time: "11 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
@@ -3929,27 +3929,27 @@
       </c>
       <c r="J61" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 58</v>
+        <v>{ id: 58</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Rainbow Stag"</v>
+        <v>, name: "Rainbow Stag"</v>
       </c>
       <c r="L61" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M61" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 6000</v>
+        <v>, value: 6000</v>
       </c>
       <c r="N61" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "7 p.m. - 8 a.m."</v>
+        <v>, time: "7 p.m. - 8 a.m."</v>
       </c>
       <c r="O61" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "June-September (Northern) / December-March (Southern)"</v>
+        <v>, season: "June-September (Northern) / December-March (Southern)"</v>
       </c>
       <c r="P61" t="str">
         <f t="shared" si="6"/>
@@ -3958,7 +3958,7 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 58, "name": "Rainbow Stag", "type": "On trees", "value": 6000, "time": "7 p.m. - 8 a.m.", "season": "June-September (Northern) / December-March (Southern)" },</v>
+        <v>{ id: 58, name: "Rainbow Stag", type: "On trees", value: 6000, time: "7 p.m. - 8 a.m.", season: "June-September (Northern) / December-March (Southern)" },</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
@@ -3982,27 +3982,27 @@
       </c>
       <c r="J62" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 59</v>
+        <v>{ id: 59</v>
       </c>
       <c r="K62" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Cyclommatus Stag"</v>
+        <v>, name: "Cyclommatus Stag"</v>
       </c>
       <c r="L62" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On coconut trees"</v>
+        <v>, type: "On coconut trees"</v>
       </c>
       <c r="M62" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 8000</v>
+        <v>, value: 8000</v>
       </c>
       <c r="N62" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O62" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P62" t="str">
         <f t="shared" si="6"/>
@@ -4011,7 +4011,7 @@
       <c r="Q62" s="2"/>
       <c r="R62" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 59, "name": "Cyclommatus Stag", "type": "On coconut trees", "value": 8000, "time": "5 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 59, name: "Cyclommatus Stag", type: "On coconut trees", value: 8000, time: "5 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
@@ -4035,27 +4035,27 @@
       </c>
       <c r="J63" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 60</v>
+        <v>{ id: 60</v>
       </c>
       <c r="K63" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Golden Stag"</v>
+        <v>, name: "Golden Stag"</v>
       </c>
       <c r="L63" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On coconut trees"</v>
+        <v>, type: "On coconut trees"</v>
       </c>
       <c r="M63" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 12000</v>
+        <v>, value: 12000</v>
       </c>
       <c r="N63" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O63" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P63" t="str">
         <f t="shared" si="6"/>
@@ -4064,7 +4064,7 @@
       <c r="Q63" s="2"/>
       <c r="R63" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 60, "name": "Golden Stag", "type": "On coconut trees", "value": 12000, "time": "5 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 60, name: "Golden Stag", type: "On coconut trees", value: 12000, time: "5 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
@@ -4088,27 +4088,27 @@
       </c>
       <c r="J64" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 61</v>
+        <v>{ id: 61</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Giraffe Stag"</v>
+        <v>, name: "Giraffe Stag"</v>
       </c>
       <c r="L64" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On coconut trees"</v>
+        <v>, type: "On coconut trees"</v>
       </c>
       <c r="M64" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 12000</v>
+        <v>, value: 12000</v>
       </c>
       <c r="N64" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O64" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P64" t="str">
         <f t="shared" si="6"/>
@@ -4117,7 +4117,7 @@
       <c r="Q64" s="2"/>
       <c r="R64" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 61, "name": "Giraffe Stag", "type": "On coconut trees", "value": 12000, "time": "5 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 61, name: "Giraffe Stag", type: "On coconut trees", value: 12000, time: "5 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
@@ -4141,27 +4141,27 @@
       </c>
       <c r="J65" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 62</v>
+        <v>{ id: 62</v>
       </c>
       <c r="K65" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Horned Dynastid"</v>
+        <v>, name: "Horned Dynastid"</v>
       </c>
       <c r="L65" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M65" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 1350</v>
+        <v>, value: 1350</v>
       </c>
       <c r="N65" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O65" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P65" t="str">
         <f t="shared" si="6"/>
@@ -4170,7 +4170,7 @@
       <c r="Q65" s="2"/>
       <c r="R65" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 62, "name": "Horned Dynastid", "type": "On trees", "value": 1350, "time": "5 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 62, name: "Horned Dynastid", type: "On trees", value: 1350, time: "5 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
@@ -4194,27 +4194,27 @@
       </c>
       <c r="J66" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 63</v>
+        <v>{ id: 63</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Horned Atlas"</v>
+        <v>, name: "Horned Atlas"</v>
       </c>
       <c r="L66" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On coconut trees"</v>
+        <v>, type: "On coconut trees"</v>
       </c>
       <c r="M66" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 8000</v>
+        <v>, value: 8000</v>
       </c>
       <c r="N66" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O66" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P66" t="str">
         <f t="shared" si="6"/>
@@ -4223,7 +4223,7 @@
       <c r="Q66" s="2"/>
       <c r="R66" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 63, "name": "Horned Atlas", "type": "On coconut trees", "value": 8000, "time": "5 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 63, name: "Horned Atlas", type: "On coconut trees", value: 8000, time: "5 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
@@ -4247,27 +4247,27 @@
       </c>
       <c r="J67" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 64</v>
+        <v>{ id: 64</v>
       </c>
       <c r="K67" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Horned Elephant"</v>
+        <v>, name: "Horned Elephant"</v>
       </c>
       <c r="L67" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On coconut trees"</v>
+        <v>, type: "On coconut trees"</v>
       </c>
       <c r="M67" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 8000</v>
+        <v>, value: 8000</v>
       </c>
       <c r="N67" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O67" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P67" t="str">
         <f t="shared" si="6"/>
@@ -4276,7 +4276,7 @@
       <c r="Q67" s="2"/>
       <c r="R67" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 64, "name": "Horned Elephant", "type": "On coconut trees", "value": 8000, "time": "5 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 64, name: "Horned Elephant", type: "On coconut trees", value: 8000, time: "5 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
@@ -4300,27 +4300,27 @@
       </c>
       <c r="J68" t="str">
         <f t="shared" si="0"/>
-        <v>{ "id": 65</v>
+        <v>{ id: 65</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="1"/>
-        <v>, "name": "Horned Herucles"</v>
+        <v>, name: "Horned Herucles"</v>
       </c>
       <c r="L68" t="str">
         <f t="shared" si="2"/>
-        <v>, "type": "On coconut trees"</v>
+        <v>, type: "On coconut trees"</v>
       </c>
       <c r="M68" t="str">
         <f t="shared" si="3"/>
-        <v>, "value": 12000</v>
+        <v>, value: 12000</v>
       </c>
       <c r="N68" t="str">
         <f t="shared" si="4"/>
-        <v>, "time": "5 p.m. - 8 a.m."</v>
+        <v>, time: "5 p.m. - 8 a.m."</v>
       </c>
       <c r="O68" t="str">
         <f t="shared" si="5"/>
-        <v>, "season": "July-August (Northern) / January-February (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-February (Southern)"</v>
       </c>
       <c r="P68" t="str">
         <f t="shared" si="6"/>
@@ -4329,7 +4329,7 @@
       <c r="Q68" s="2"/>
       <c r="R68" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>{ "id": 65, "name": "Horned Herucles", "type": "On coconut trees", "value": 12000, "time": "5 p.m. - 8 a.m.", "season": "July-August (Northern) / January-February (Southern)" },</v>
+        <v>{ id: 65, name: "Horned Herucles", type: "On coconut trees", value: 12000, time: "5 p.m. - 8 a.m.", season: "July-August (Northern) / January-February (Southern)" },</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
@@ -4353,27 +4353,27 @@
       </c>
       <c r="J69" t="str">
         <f t="shared" ref="J69:J83" si="8">J$1&amp;A69</f>
-        <v>{ "id": 66</v>
+        <v>{ id: 66</v>
       </c>
       <c r="K69" t="str">
         <f t="shared" ref="K69:K83" si="9">K$1&amp;""""&amp;B69&amp;""""</f>
-        <v>, "name": "Walking Stick"</v>
+        <v>, name: "Walking Stick"</v>
       </c>
       <c r="L69" t="str">
         <f t="shared" ref="L69:L83" si="10">L$1&amp;""""&amp;C69&amp;""""</f>
-        <v>, "type": "On trees"</v>
+        <v>, type: "On trees"</v>
       </c>
       <c r="M69" t="str">
         <f t="shared" ref="M69:M83" si="11">M$1&amp;D69</f>
-        <v>, "value": 600</v>
+        <v>, value: 600</v>
       </c>
       <c r="N69" t="str">
         <f t="shared" ref="N69:N83" si="12">N$1&amp;""""&amp;E69&amp;""""</f>
-        <v>, "time": "4 a.m. - 8 a.m., 5 p.m. - 7 p.m."</v>
+        <v>, time: "4 a.m. - 8 a.m., 5 p.m. - 7 p.m."</v>
       </c>
       <c r="O69" t="str">
         <f t="shared" ref="O69:O83" si="13">O$1&amp;""""&amp;F69&amp;""""</f>
-        <v>, "season": "July-November (Northern) / January-May (Southern)"</v>
+        <v>, season: "July-November (Northern) / January-May (Southern)"</v>
       </c>
       <c r="P69" t="str">
         <f t="shared" ref="P69:P83" si="14">P$1</f>
@@ -4382,7 +4382,7 @@
       <c r="Q69" s="2"/>
       <c r="R69" s="2" t="str">
         <f t="shared" ref="R69:R83" si="15">J69&amp;K69&amp;L69&amp;M69&amp;N69&amp;O69&amp;P69</f>
-        <v>{ "id": 66, "name": "Walking Stick", "type": "On trees", "value": 600, "time": "4 a.m. - 8 a.m., 5 p.m. - 7 p.m.", "season": "July-November (Northern) / January-May (Southern)" },</v>
+        <v>{ id: 66, name: "Walking Stick", type: "On trees", value: 600, time: "4 a.m. - 8 a.m., 5 p.m. - 7 p.m.", season: "July-November (Northern) / January-May (Southern)" },</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
@@ -4406,27 +4406,27 @@
       </c>
       <c r="J70" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 67</v>
+        <v>{ id: 67</v>
       </c>
       <c r="K70" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Walking Leaf"</v>
+        <v>, name: "Walking Leaf"</v>
       </c>
       <c r="L70" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "Near trees, disguised as furniture leaf"</v>
+        <v>, type: "Near trees, disguised as furniture leaf"</v>
       </c>
       <c r="M70" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 600</v>
+        <v>, value: 600</v>
       </c>
       <c r="N70" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O70" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "July-August (Northern) / January-March (Southern)"</v>
+        <v>, season: "July-August (Northern) / January-March (Southern)"</v>
       </c>
       <c r="P70" t="str">
         <f t="shared" si="14"/>
@@ -4435,7 +4435,7 @@
       <c r="Q70" s="2"/>
       <c r="R70" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 67, "name": "Walking Leaf", "type": "Near trees, disguised as furniture leaf", "value": 600, "time": "All day", "season": "July-August (Northern) / January-March (Southern)" },</v>
+        <v>{ id: 67, name: "Walking Leaf", type: "Near trees, disguised as furniture leaf", value: 600, time: "All day", season: "July-August (Northern) / January-March (Southern)" },</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
@@ -4459,27 +4459,27 @@
       </c>
       <c r="J71" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 68</v>
+        <v>{ id: 68</v>
       </c>
       <c r="K71" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Bagworm"</v>
+        <v>, name: "Bagworm"</v>
       </c>
       <c r="L71" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "Falls from shaking trees"</v>
+        <v>, type: "Falls from shaking trees"</v>
       </c>
       <c r="M71" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 600</v>
+        <v>, value: 600</v>
       </c>
       <c r="N71" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O71" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P71" t="str">
         <f t="shared" si="14"/>
@@ -4488,7 +4488,7 @@
       <c r="Q71" s="2"/>
       <c r="R71" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 68, "name": "Bagworm", "type": "Falls from shaking trees", "value": 600, "time": "All day", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 68, name: "Bagworm", type: "Falls from shaking trees", value: 600, time: "All day", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
@@ -4512,27 +4512,27 @@
       </c>
       <c r="J72" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 69</v>
+        <v>{ id: 69</v>
       </c>
       <c r="K72" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Ant"</v>
+        <v>, name: "Ant"</v>
       </c>
       <c r="L72" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "On rotten food"</v>
+        <v>, type: "On rotten food"</v>
       </c>
       <c r="M72" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 80</v>
+        <v>, value: 80</v>
       </c>
       <c r="N72" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O72" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P72" t="str">
         <f t="shared" si="14"/>
@@ -4541,7 +4541,7 @@
       <c r="Q72" s="2"/>
       <c r="R72" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 69, "name": "Ant", "type": "On rotten food", "value": 80, "time": "All day", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 69, name: "Ant", type: "On rotten food", value: 80, time: "All day", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
@@ -4565,27 +4565,27 @@
       </c>
       <c r="J73" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 70</v>
+        <v>{ id: 70</v>
       </c>
       <c r="K73" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Hermit Crab"</v>
+        <v>, name: "Hermit Crab"</v>
       </c>
       <c r="L73" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "Beach"</v>
+        <v>, type: "Beach"</v>
       </c>
       <c r="M73" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 1000</v>
+        <v>, value: 1000</v>
       </c>
       <c r="N73" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "7 p.m. - 8 a.m."</v>
+        <v>, time: "7 p.m. - 8 a.m."</v>
       </c>
       <c r="O73" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P73" t="str">
         <f t="shared" si="14"/>
@@ -4594,7 +4594,7 @@
       <c r="Q73" s="2"/>
       <c r="R73" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 70, "name": "Hermit Crab", "type": "Beach", "value": 1000, "time": "7 p.m. - 8 a.m.", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 70, name: "Hermit Crab", type: "Beach", value: 1000, time: "7 p.m. - 8 a.m.", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
@@ -4618,27 +4618,27 @@
       </c>
       <c r="J74" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 71</v>
+        <v>{ id: 71</v>
       </c>
       <c r="K74" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Wharf Roach"</v>
+        <v>, name: "Wharf Roach"</v>
       </c>
       <c r="L74" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "On rocks at beach"</v>
+        <v>, type: "On rocks at beach"</v>
       </c>
       <c r="M74" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 200</v>
+        <v>, value: 200</v>
       </c>
       <c r="N74" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O74" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P74" t="str">
         <f t="shared" si="14"/>
@@ -4647,7 +4647,7 @@
       <c r="Q74" s="2"/>
       <c r="R74" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 71, "name": "Wharf Roach", "type": "On rocks at beach", "value": 200, "time": "All day", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 71, name: "Wharf Roach", type: "On rocks at beach", value: 200, time: "All day", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
@@ -4671,27 +4671,27 @@
       </c>
       <c r="J75" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 72</v>
+        <v>{ id: 72</v>
       </c>
       <c r="K75" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Fly"</v>
+        <v>, name: "Fly"</v>
       </c>
       <c r="L75" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "On trash items"</v>
+        <v>, type: "On trash items"</v>
       </c>
       <c r="M75" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 60</v>
+        <v>, value: 60</v>
       </c>
       <c r="N75" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O75" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P75" t="str">
         <f t="shared" si="14"/>
@@ -4700,7 +4700,7 @@
       <c r="Q75" s="2"/>
       <c r="R75" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 72, "name": "Fly", "type": "On trash items", "value": 60, "time": "All day", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 72, name: "Fly", type: "On trash items", value: 60, time: "All day", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
@@ -4724,27 +4724,27 @@
       </c>
       <c r="J76" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 73</v>
+        <v>{ id: 73</v>
       </c>
       <c r="K76" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Mosquito"</v>
+        <v>, name: "Mosquito"</v>
       </c>
       <c r="L76" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "Flying"</v>
+        <v>, type: "Flying"</v>
       </c>
       <c r="M76" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 130</v>
+        <v>, value: 130</v>
       </c>
       <c r="N76" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "5 p.m. - 4 a.m."</v>
+        <v>, time: "5 p.m. - 4 a.m."</v>
       </c>
       <c r="O76" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "June-September (Northern) / December-March (Southern)"</v>
+        <v>, season: "June-September (Northern) / December-March (Southern)"</v>
       </c>
       <c r="P76" t="str">
         <f t="shared" si="14"/>
@@ -4753,7 +4753,7 @@
       <c r="Q76" s="2"/>
       <c r="R76" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 73, "name": "Mosquito", "type": "Flying", "value": 130, "time": "5 p.m. - 4 a.m.", "season": "June-September (Northern) / December-March (Southern)" },</v>
+        <v>{ id: 73, name: "Mosquito", type: "Flying", value: 130, time: "5 p.m. - 4 a.m.", season: "June-September (Northern) / December-March (Southern)" },</v>
       </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
@@ -4777,27 +4777,27 @@
       </c>
       <c r="J77" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 74</v>
+        <v>{ id: 74</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Flea"</v>
+        <v>, name: "Flea"</v>
       </c>
       <c r="L77" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "On villagers"</v>
+        <v>, type: "On villagers"</v>
       </c>
       <c r="M77" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 70</v>
+        <v>, value: 70</v>
       </c>
       <c r="N77" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O77" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "April-November (Northern) / October-May (Southern)"</v>
+        <v>, season: "April-November (Northern) / October-May (Southern)"</v>
       </c>
       <c r="P77" t="str">
         <f t="shared" si="14"/>
@@ -4806,7 +4806,7 @@
       <c r="Q77" s="2"/>
       <c r="R77" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 74, "name": "Flea", "type": "On villagers", "value": 70, "time": "All day", "season": "April-November (Northern) / October-May (Southern)" },</v>
+        <v>{ id: 74, name: "Flea", type: "On villagers", value: 70, time: "All day", season: "April-November (Northern) / October-May (Southern)" },</v>
       </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
@@ -4830,27 +4830,27 @@
       </c>
       <c r="J78" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 75</v>
+        <v>{ id: 75</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Snail"</v>
+        <v>, name: "Snail"</v>
       </c>
       <c r="L78" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "On rocks (raining)"</v>
+        <v>, type: "On rocks (raining)"</v>
       </c>
       <c r="M78" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 250</v>
+        <v>, value: 250</v>
       </c>
       <c r="N78" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "All day"</v>
+        <v>, time: "All day"</v>
       </c>
       <c r="O78" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P78" t="str">
         <f t="shared" si="14"/>
@@ -4859,7 +4859,7 @@
       <c r="Q78" s="2"/>
       <c r="R78" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 75, "name": "Snail", "type": "On rocks (raining)", "value": 250, "time": "All day", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 75, name: "Snail", type: "On rocks (raining)", value: 250, time: "All day", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
@@ -4883,27 +4883,27 @@
       </c>
       <c r="J79" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 76</v>
+        <v>{ id: 76</v>
       </c>
       <c r="K79" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Pill Bug"</v>
+        <v>, name: "Pill Bug"</v>
       </c>
       <c r="L79" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "Hit rocks"</v>
+        <v>, type: "Hit rocks"</v>
       </c>
       <c r="M79" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 250</v>
+        <v>, value: 250</v>
       </c>
       <c r="N79" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "11 p.m. - 4 p.m."</v>
+        <v>, time: "11 p.m. - 4 p.m."</v>
       </c>
       <c r="O79" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "September-June (Northern) / March-December (Southern)"</v>
+        <v>, season: "September-June (Northern) / March-December (Southern)"</v>
       </c>
       <c r="P79" t="str">
         <f t="shared" si="14"/>
@@ -4912,7 +4912,7 @@
       <c r="Q79" s="2"/>
       <c r="R79" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 76, "name": "Pill Bug", "type": "Hit rocks", "value": 250, "time": "11 p.m. - 4 p.m.", "season": "September-June (Northern) / March-December (Southern)" },</v>
+        <v>{ id: 76, name: "Pill Bug", type: "Hit rocks", value: 250, time: "11 p.m. - 4 p.m.", season: "September-June (Northern) / March-December (Southern)" },</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
@@ -4936,27 +4936,27 @@
       </c>
       <c r="J80" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 77</v>
+        <v>{ id: 77</v>
       </c>
       <c r="K80" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Centipede"</v>
+        <v>, name: "Centipede"</v>
       </c>
       <c r="L80" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "Hit rocks"</v>
+        <v>, type: "Hit rocks"</v>
       </c>
       <c r="M80" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 300</v>
+        <v>, value: 300</v>
       </c>
       <c r="N80" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "4 p.m. - 11 p.m."</v>
+        <v>, time: "4 p.m. - 11 p.m."</v>
       </c>
       <c r="O80" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "September-June (Northern) / March-December (Southern)"</v>
+        <v>, season: "September-June (Northern) / March-December (Southern)"</v>
       </c>
       <c r="P80" t="str">
         <f t="shared" si="14"/>
@@ -4965,7 +4965,7 @@
       <c r="Q80" s="2"/>
       <c r="R80" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 77, "name": "Centipede", "type": "Hit rocks", "value": 300, "time": "4 p.m. - 11 p.m.", "season": "September-June (Northern) / March-December (Southern)" },</v>
+        <v>{ id: 77, name: "Centipede", type: "Hit rocks", value: 300, time: "4 p.m. - 11 p.m.", season: "September-June (Northern) / March-December (Southern)" },</v>
       </c>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
@@ -4989,27 +4989,27 @@
       </c>
       <c r="J81" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 78</v>
+        <v>{ id: 78</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Spider"</v>
+        <v>, name: "Spider"</v>
       </c>
       <c r="L81" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "Falls from shaking trees"</v>
+        <v>, type: "Falls from shaking trees"</v>
       </c>
       <c r="M81" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 480</v>
+        <v>, value: 480</v>
       </c>
       <c r="N81" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "7 p.m. - 8 a.m."</v>
+        <v>, time: "7 p.m. - 8 a.m."</v>
       </c>
       <c r="O81" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "Year-round (Northern and Southern)"</v>
+        <v>, season: "Year-round (Northern and Southern)"</v>
       </c>
       <c r="P81" t="str">
         <f t="shared" si="14"/>
@@ -5018,7 +5018,7 @@
       <c r="Q81" s="2"/>
       <c r="R81" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 78, "name": "Spider", "type": "Falls from shaking trees", "value": 480, "time": "7 p.m. - 8 a.m.", "season": "Year-round (Northern and Southern)" },</v>
+        <v>{ id: 78, name: "Spider", type: "Falls from shaking trees", value: 480, time: "7 p.m. - 8 a.m.", season: "Year-round (Northern and Southern)" },</v>
       </c>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
@@ -5042,27 +5042,27 @@
       </c>
       <c r="J82" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 79</v>
+        <v>{ id: 79</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Tarantula"</v>
+        <v>, name: "Tarantula"</v>
       </c>
       <c r="L82" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M82" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 8000</v>
+        <v>, value: 8000</v>
       </c>
       <c r="N82" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "7 p.m. - 4 a.m."</v>
+        <v>, time: "7 p.m. - 4 a.m."</v>
       </c>
       <c r="O82" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "November-April (Northern) / May-October (Southern)"</v>
+        <v>, season: "November-April (Northern) / May-October (Southern)"</v>
       </c>
       <c r="P82" t="str">
         <f t="shared" si="14"/>
@@ -5071,7 +5071,7 @@
       <c r="Q82" s="2"/>
       <c r="R82" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 79, "name": "Tarantula", "type": "On ground", "value": 8000, "time": "7 p.m. - 4 a.m.", "season": "November-April (Northern) / May-October (Southern)" },</v>
+        <v>{ id: 79, name: "Tarantula", type: "On ground", value: 8000, time: "7 p.m. - 4 a.m.", season: "November-April (Northern) / May-October (Southern)" },</v>
       </c>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
@@ -5095,27 +5095,27 @@
       </c>
       <c r="J83" t="str">
         <f t="shared" si="8"/>
-        <v>{ "id": 80</v>
+        <v>{ id: 80</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="9"/>
-        <v>, "name": "Scorpion"</v>
+        <v>, name: "Scorpion"</v>
       </c>
       <c r="L83" t="str">
         <f t="shared" si="10"/>
-        <v>, "type": "On ground"</v>
+        <v>, type: "On ground"</v>
       </c>
       <c r="M83" t="str">
         <f t="shared" si="11"/>
-        <v>, "value": 8000</v>
+        <v>, value: 8000</v>
       </c>
       <c r="N83" t="str">
         <f t="shared" si="12"/>
-        <v>, "time": "7 p.m. - 4 a.m."</v>
+        <v>, time: "7 p.m. - 4 a.m."</v>
       </c>
       <c r="O83" t="str">
         <f t="shared" si="13"/>
-        <v>, "season": "May-October (Northern) / November-April (Southern)"</v>
+        <v>, season: "May-October (Northern) / November-April (Southern)"</v>
       </c>
       <c r="P83" t="str">
         <f t="shared" si="14"/>
@@ -5124,7 +5124,7 @@
       <c r="Q83" s="2"/>
       <c r="R83" s="2" t="str">
         <f t="shared" si="15"/>
-        <v>{ "id": 80, "name": "Scorpion", "type": "On ground", "value": 8000, "time": "7 p.m. - 4 a.m.", "season": "May-October (Northern) / November-April (Southern)" },</v>
+        <v>{ id: 80, name: "Scorpion", type: "On ground", value: 8000, time: "7 p.m. - 4 a.m.", season: "May-October (Northern) / November-April (Southern)" },</v>
       </c>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>